<commit_message>
Ticket 86 - Move, remove, and copy existing Excel hyperlinks.
</commit_message>
<xml_diff>
--- a/jett-core/templates/HyperlinkTagTemplate.xlsx
+++ b/jett-core/templates/HyperlinkTagTemplate.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svn\jett\jett-core\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="22035" windowHeight="11565"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="22040" windowHeight="11570"/>
   </bookViews>
   <sheets>
     <sheet name="Hyperlinks" sheetId="1" r:id="rId1"/>
     <sheet name="Target Sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Shift" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Hyperlinks!</t>
   </si>
@@ -74,12 +80,30 @@
       <t>"/&gt;</t>
     </r>
   </si>
+  <si>
+    <t>Shift!</t>
+  </si>
+  <si>
+    <t>Copy!</t>
+  </si>
+  <si>
+    <t>&lt;jt:for var="i" start="1" end="10"&gt;</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>&lt;/jt:for&gt;</t>
+  </si>
+  <si>
+    <t>JETT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +115,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,13 +145,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -132,6 +167,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -180,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,9 +251,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,6 +303,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,22 +500,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -460,9 +532,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -470,4 +542,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>